<commit_message>
Updated gj.py to use new functions
</commit_message>
<xml_diff>
--- a/Results/Gj.xlsx
+++ b/Results/Gj.xlsx
@@ -522,7 +522,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B2:O1268"/>
+  <dimension ref="B2:Q1268"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N2" sqref="N2:O3"/>
@@ -704,6 +704,14 @@
       <c r="O4" t="n">
         <v>0.07082257092231303</v>
       </c>
+      <c r="P4" t="inlineStr">
+        <is>
+          <t>MEEFEITIH</t>
+        </is>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.06572004464283529</v>
+      </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
@@ -762,6 +770,14 @@
       <c r="O5" t="n">
         <v>0.07060755523038587</v>
       </c>
+      <c r="P5" t="inlineStr">
+        <is>
+          <t>MMEEFEITI</t>
+        </is>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.06527797505648819</v>
+      </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
@@ -820,6 +836,14 @@
       <c r="O6" t="n">
         <v>0.06904986855818178</v>
       </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>EEFEITIHR</t>
+        </is>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.06380417009806016</v>
+      </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
@@ -878,6 +902,14 @@
       <c r="O7" t="n">
         <v>0.06880935871191145</v>
       </c>
+      <c r="P7" t="inlineStr">
+        <is>
+          <t>EMMEEFEIT</t>
+        </is>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.06364996497479281</v>
+      </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
@@ -936,6 +968,14 @@
       <c r="O8" t="n">
         <v>0.06859841296596596</v>
       </c>
+      <c r="P8" t="inlineStr">
+        <is>
+          <t>LLGYIEEIK</t>
+        </is>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.0622395860008393</v>
+      </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
@@ -994,6 +1034,14 @@
       <c r="O9" t="n">
         <v>0.06838297605222271</v>
       </c>
+      <c r="P9" t="inlineStr">
+        <is>
+          <t>EFEITIHRP</t>
+        </is>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.06178846466875153</v>
+      </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
@@ -1052,6 +1100,14 @@
       <c r="O10" t="n">
         <v>0.06827794400550122</v>
       </c>
+      <c r="P10" t="inlineStr">
+        <is>
+          <t>LGYIEEIKF</t>
+        </is>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.06107992215464007</v>
+      </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
@@ -1110,6 +1166,14 @@
       <c r="O11" t="n">
         <v>0.06757359289993534</v>
       </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>GYIEEIKFA</t>
+        </is>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.05960548647190239</v>
+      </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
@@ -1168,6 +1232,14 @@
       <c r="O12" t="n">
         <v>0.06685702587544183</v>
       </c>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>IAGAANWTN</t>
+        </is>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.05923832575224897</v>
+      </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
@@ -1226,6 +1298,14 @@
       <c r="O13" t="n">
         <v>0.06618873742152061</v>
       </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>AGAANWTNG</t>
+        </is>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.05922711262346664</v>
+      </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
@@ -1284,6 +1364,14 @@
       <c r="O14" t="n">
         <v>0.06570132122158689</v>
       </c>
+      <c r="P14" t="inlineStr">
+        <is>
+          <t>GKIHILAFK</t>
+        </is>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.05835021713324512</v>
+      </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
@@ -1342,6 +1430,14 @@
       <c r="O15" t="n">
         <v>0.0655505716292067</v>
       </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>GLLGYIEEI</t>
+        </is>
+      </c>
+      <c r="Q15" t="n">
+        <v>0.05821989058040858</v>
+      </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
@@ -1400,6 +1496,14 @@
       <c r="O16" t="n">
         <v>0.06510458538868411</v>
       </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>FEITIHRPK</t>
+        </is>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.05745634206169023</v>
+      </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
@@ -1458,6 +1562,14 @@
       <c r="O17" t="n">
         <v>0.06485017176254609</v>
       </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>DGKIHILAF</t>
+        </is>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.05717046465673384</v>
+      </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
@@ -1516,6 +1628,14 @@
       <c r="O18" t="n">
         <v>0.0648477433932248</v>
       </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>YIEEIKFAY</t>
+        </is>
+      </c>
+      <c r="Q18" t="n">
+        <v>0.05703672622349282</v>
+      </c>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
@@ -1574,6 +1694,14 @@
       <c r="O19" t="n">
         <v>0.06415869079842586</v>
       </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>GIAGAANWT</t>
+        </is>
+      </c>
+      <c r="Q19" t="n">
+        <v>0.05688675962120156</v>
+      </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
@@ -1632,6 +1760,14 @@
       <c r="O20" t="n">
         <v>0.06384423571817785</v>
       </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>ESGIAGAAN</t>
+        </is>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.0568722155900105</v>
+      </c>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
@@ -1690,6 +1826,14 @@
       <c r="O21" t="n">
         <v>0.06307412476601097</v>
       </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>AAARGTITL</t>
+        </is>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.05673188251400917</v>
+      </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
@@ -1748,6 +1892,14 @@
       <c r="O22" t="n">
         <v>0.06295991696623912</v>
       </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>AARGTITLT</t>
+        </is>
+      </c>
+      <c r="Q22" t="n">
+        <v>0.05579545683740722</v>
+      </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
@@ -1806,6 +1958,14 @@
       <c r="O23" t="n">
         <v>0.0629253820402747</v>
       </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>AAAARGTIT</t>
+        </is>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.05567950941874505</v>
+      </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
@@ -1864,6 +2024,14 @@
       <c r="O24" t="n">
         <v>0.06280965515855773</v>
       </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>ARGTITLTK</t>
+        </is>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.05545172428175964</v>
+      </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
@@ -1922,6 +2090,14 @@
       <c r="O25" t="n">
         <v>0.06262136540418681</v>
       </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>DLTELLFTY</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.05502042417226133</v>
+      </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
@@ -1980,6 +2156,14 @@
       <c r="O26" t="n">
         <v>0.0621227470494637</v>
       </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>AESGIAGAA</t>
+        </is>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.05484182214837124</v>
+      </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
@@ -2038,6 +2222,14 @@
       <c r="O27" t="n">
         <v>0.06202938817774351</v>
       </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>REMMEEFEI</t>
+        </is>
+      </c>
+      <c r="Q27" t="n">
+        <v>0.05442942614185246</v>
+      </c>
     </row>
     <row r="28">
       <c r="B28" t="inlineStr">
@@ -2096,6 +2288,14 @@
       <c r="O28" t="n">
         <v>0.06174261383226515</v>
       </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>KIHILAFKN</t>
+        </is>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.054398745973054</v>
+      </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
@@ -2154,6 +2354,14 @@
       <c r="O29" t="n">
         <v>0.06123251367695647</v>
       </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>EGLLGYIEE</t>
+        </is>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.05406531269718829</v>
+      </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
@@ -2212,6 +2420,14 @@
       <c r="O30" t="n">
         <v>0.06123058606074101</v>
       </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>IEEIKFAYS</t>
+        </is>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.05391825530687247</v>
+      </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
@@ -2270,6 +2486,14 @@
       <c r="O31" t="n">
         <v>0.06105495759838682</v>
       </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>GDLTELLFT</t>
+        </is>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.05375791813564762</v>
+      </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
@@ -2328,6 +2552,14 @@
       <c r="O32" t="n">
         <v>0.06060377563668191</v>
       </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>YSLEHAESG</t>
+        </is>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.05362787166492214</v>
+      </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
@@ -2386,6 +2618,14 @@
       <c r="O33" t="n">
         <v>0.06049409544432425</v>
       </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>EHAESGIAG</t>
+        </is>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.05341597290906665</v>
+      </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
@@ -2444,6 +2684,14 @@
       <c r="O34" t="n">
         <v>0.06043685827202993</v>
       </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>TPAAAARGT</t>
+        </is>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.05333119690076816</v>
+      </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
@@ -2502,6 +2750,14 @@
       <c r="O35" t="n">
         <v>0.06038418161332556</v>
       </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>PAAAARGTI</t>
+        </is>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.05332114644339227</v>
+      </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
@@ -2560,6 +2816,14 @@
       <c r="O36" t="n">
         <v>0.06037102134907295</v>
       </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>SGIAGAANW</t>
+        </is>
+      </c>
+      <c r="Q36" t="n">
+        <v>0.0532573723988755</v>
+      </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
@@ -2618,6 +2882,14 @@
       <c r="O37" t="n">
         <v>0.06004341241649458</v>
       </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>GYSLEHAES</t>
+        </is>
+      </c>
+      <c r="Q37" t="n">
+        <v>0.05317635366526818</v>
+      </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
@@ -2676,6 +2948,14 @@
       <c r="O38" t="n">
         <v>0.059918630452204</v>
       </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>FEKVLITHM</t>
+        </is>
+      </c>
+      <c r="Q38" t="n">
+        <v>0.05304344777516209</v>
+      </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
@@ -2734,6 +3014,14 @@
       <c r="O39" t="n">
         <v>0.05986429204265385</v>
       </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>VVQEGHDGK</t>
+        </is>
+      </c>
+      <c r="Q39" t="n">
+        <v>0.05304340963382105</v>
+      </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
@@ -2792,6 +3080,14 @@
       <c r="O40" t="n">
         <v>0.05967209383036019</v>
       </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>LTPAAAARG</t>
+        </is>
+      </c>
+      <c r="Q40" t="n">
+        <v>0.05276560147003617</v>
+      </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
@@ -2850,6 +3146,14 @@
       <c r="O41" t="n">
         <v>0.05960950032142061</v>
       </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>HDGKIHILA</t>
+        </is>
+      </c>
+      <c r="Q41" t="n">
+        <v>0.0526819631475348</v>
+      </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
@@ -2908,6 +3212,14 @@
       <c r="O42" t="n">
         <v>0.05949902291195368</v>
       </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>LTELLFTYK</t>
+        </is>
+      </c>
+      <c r="Q42" t="n">
+        <v>0.05267431343811571</v>
+      </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
@@ -2966,6 +3278,14 @@
       <c r="O43" t="n">
         <v>0.05948983054709189</v>
       </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>LEHAESGIA</t>
+        </is>
+      </c>
+      <c r="Q43" t="n">
+        <v>0.0524016233403759</v>
+      </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
@@ -3024,6 +3344,14 @@
       <c r="O44" t="n">
         <v>0.05939411757458836</v>
       </c>
+      <c r="P44" t="inlineStr">
+        <is>
+          <t>GHDGKIHIL</t>
+        </is>
+      </c>
+      <c r="Q44" t="n">
+        <v>0.05240073753363172</v>
+      </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
@@ -3082,6 +3410,14 @@
       <c r="O45" t="n">
         <v>0.05931222695955147</v>
       </c>
+      <c r="P45" t="inlineStr">
+        <is>
+          <t>DSNGIKEGL</t>
+        </is>
+      </c>
+      <c r="Q45" t="n">
+        <v>0.05225886368830376</v>
+      </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
@@ -3140,6 +3476,14 @@
       <c r="O46" t="n">
         <v>0.05929519478975719</v>
       </c>
+      <c r="P46" t="inlineStr">
+        <is>
+          <t>EITIHRPKT</t>
+        </is>
+      </c>
+      <c r="Q46" t="n">
+        <v>0.0521463670926493</v>
+      </c>
     </row>
     <row r="47">
       <c r="B47" t="inlineStr">
@@ -3198,6 +3542,14 @@
       <c r="O47" t="n">
         <v>0.05926207520248875</v>
       </c>
+      <c r="P47" t="inlineStr">
+        <is>
+          <t>PKTDTTGGD</t>
+        </is>
+      </c>
+      <c r="Q47" t="n">
+        <v>0.05213246486801888</v>
+      </c>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
@@ -3256,6 +3608,14 @@
       <c r="O48" t="n">
         <v>0.05924533558973342</v>
       </c>
+      <c r="P48" t="inlineStr">
+        <is>
+          <t>KTDTTGGDL</t>
+        </is>
+      </c>
+      <c r="Q48" t="n">
+        <v>0.05212624755155061</v>
+      </c>
     </row>
     <row r="49">
       <c r="B49" t="inlineStr">
@@ -3314,6 +3674,14 @@
       <c r="O49" t="n">
         <v>0.05922818520389227</v>
       </c>
+      <c r="P49" t="inlineStr">
+        <is>
+          <t>KTQGEIKGS</t>
+        </is>
+      </c>
+      <c r="Q49" t="n">
+        <v>0.05212256497689984</v>
+      </c>
     </row>
     <row r="50">
       <c r="B50" t="inlineStr">
@@ -3372,6 +3740,14 @@
       <c r="O50" t="n">
         <v>0.05922413515187096</v>
       </c>
+      <c r="P50" t="inlineStr">
+        <is>
+          <t>TTGGDLTEL</t>
+        </is>
+      </c>
+      <c r="Q50" t="n">
+        <v>0.0520317326370146</v>
+      </c>
     </row>
     <row r="51">
       <c r="B51" t="inlineStr">
@@ -3430,6 +3806,14 @@
       <c r="O51" t="n">
         <v>0.05917461167450602</v>
       </c>
+      <c r="P51" t="inlineStr">
+        <is>
+          <t>SNGIKEGLL</t>
+        </is>
+      </c>
+      <c r="Q51" t="n">
+        <v>0.05201514018893391</v>
+      </c>
     </row>
     <row r="52">
       <c r="B52" t="inlineStr">
@@ -3488,6 +3872,14 @@
       <c r="O52" t="n">
         <v>0.05917458542021397</v>
       </c>
+      <c r="P52" t="inlineStr">
+        <is>
+          <t>HAESGIAGA</t>
+        </is>
+      </c>
+      <c r="Q52" t="n">
+        <v>0.05181961920190777</v>
+      </c>
     </row>
     <row r="53">
       <c r="B53" t="inlineStr">
@@ -3546,6 +3938,14 @@
       <c r="O53" t="n">
         <v>0.05917302247141442</v>
       </c>
+      <c r="P53" t="inlineStr">
+        <is>
+          <t>TGGDLTELL</t>
+        </is>
+      </c>
+      <c r="Q53" t="n">
+        <v>0.05179597659350441</v>
+      </c>
     </row>
     <row r="54">
       <c r="B54" t="inlineStr">
@@ -3604,6 +4004,14 @@
       <c r="O54" t="n">
         <v>0.05909596463133557</v>
       </c>
+      <c r="P54" t="inlineStr">
+        <is>
+          <t>RGTITLTKE</t>
+        </is>
+      </c>
+      <c r="Q54" t="n">
+        <v>0.05175292829540754</v>
+      </c>
     </row>
     <row r="55">
       <c r="B55" t="inlineStr">
@@ -3662,6 +4070,14 @@
       <c r="O55" t="n">
         <v>0.05904950953804187</v>
       </c>
+      <c r="P55" t="inlineStr">
+        <is>
+          <t>EKVLITHMD</t>
+        </is>
+      </c>
+      <c r="Q55" t="n">
+        <v>0.05174443887591526</v>
+      </c>
     </row>
     <row r="56">
       <c r="B56" t="inlineStr">
@@ -3720,6 +4136,14 @@
       <c r="O56" t="n">
         <v>0.05902464131887444</v>
       </c>
+      <c r="P56" t="inlineStr">
+        <is>
+          <t>YKFEKVLIT</t>
+        </is>
+      </c>
+      <c r="Q56" t="n">
+        <v>0.0513844918242553</v>
+      </c>
     </row>
     <row r="57">
       <c r="B57" t="inlineStr">
@@ -3778,6 +4202,14 @@
       <c r="O57" t="n">
         <v>0.05901544274700714</v>
       </c>
+      <c r="P57" t="inlineStr">
+        <is>
+          <t>GLTPAAAAR</t>
+        </is>
+      </c>
+      <c r="Q57" t="n">
+        <v>0.05132097010488448</v>
+      </c>
     </row>
     <row r="58">
       <c r="B58" t="inlineStr">
@@ -3836,6 +4268,14 @@
       <c r="O58" t="n">
         <v>0.05891876433370929</v>
       </c>
+      <c r="P58" t="inlineStr">
+        <is>
+          <t>RLQEGLTPA</t>
+        </is>
+      </c>
+      <c r="Q58" t="n">
+        <v>0.05128662152718959</v>
+      </c>
     </row>
     <row r="59">
       <c r="B59" t="inlineStr">
@@ -3894,6 +4334,14 @@
       <c r="O59" t="n">
         <v>0.05890323014916267</v>
       </c>
+      <c r="P59" t="inlineStr">
+        <is>
+          <t>SLEHAESGI</t>
+        </is>
+      </c>
+      <c r="Q59" t="n">
+        <v>0.05118052802081148</v>
+      </c>
     </row>
     <row r="60">
       <c r="B60" t="inlineStr">
@@ -3952,6 +4400,14 @@
       <c r="O60" t="n">
         <v>0.05889492164729602</v>
       </c>
+      <c r="P60" t="inlineStr">
+        <is>
+          <t>KVLITHMDQ</t>
+        </is>
+      </c>
+      <c r="Q60" t="n">
+        <v>0.05115509530012802</v>
+      </c>
     </row>
     <row r="61">
       <c r="B61" t="inlineStr">
@@ -4010,6 +4466,14 @@
       <c r="O61" t="n">
         <v>0.05888182111277306</v>
       </c>
+      <c r="P61" t="inlineStr">
+        <is>
+          <t>TDTTGGDLT</t>
+        </is>
+      </c>
+      <c r="Q61" t="n">
+        <v>0.0511509484222384</v>
+      </c>
     </row>
     <row r="62">
       <c r="B62" t="inlineStr">
@@ -4068,6 +4532,14 @@
       <c r="O62" t="n">
         <v>0.05881585515289398</v>
       </c>
+      <c r="P62" t="inlineStr">
+        <is>
+          <t>GGDLTELLF</t>
+        </is>
+      </c>
+      <c r="Q62" t="n">
+        <v>0.05101773968427599</v>
+      </c>
     </row>
     <row r="63">
       <c r="B63" t="inlineStr">
@@ -4126,6 +4598,14 @@
       <c r="O63" t="n">
         <v>0.05871833480271599</v>
       </c>
+      <c r="P63" t="inlineStr">
+        <is>
+          <t>ELLFTYKFE</t>
+        </is>
+      </c>
+      <c r="Q63" t="n">
+        <v>0.05089841314185004</v>
+      </c>
     </row>
     <row r="64">
       <c r="B64" t="inlineStr">
@@ -4184,6 +4664,14 @@
       <c r="O64" t="n">
         <v>0.0586654182141816</v>
       </c>
+      <c r="P64" t="inlineStr">
+        <is>
+          <t>KGKTQGEIK</t>
+        </is>
+      </c>
+      <c r="Q64" t="n">
+        <v>0.05087163342982749</v>
+      </c>
     </row>
     <row r="65">
       <c r="B65" t="inlineStr">
@@ -4242,6 +4730,14 @@
       <c r="O65" t="n">
         <v>0.05857715369505054</v>
       </c>
+      <c r="P65" t="inlineStr">
+        <is>
+          <t>LLFTYKFEK</t>
+        </is>
+      </c>
+      <c r="Q65" t="n">
+        <v>0.05085577143521737</v>
+      </c>
     </row>
     <row r="66">
       <c r="B66" t="inlineStr">
@@ -4300,6 +4796,14 @@
       <c r="O66" t="n">
         <v>0.05847460182524214</v>
       </c>
+      <c r="P66" t="inlineStr">
+        <is>
+          <t>EGLTPAAAA</t>
+        </is>
+      </c>
+      <c r="Q66" t="n">
+        <v>0.05081461334159701</v>
+      </c>
     </row>
     <row r="67">
       <c r="B67" t="inlineStr">
@@ -4358,6 +4862,14 @@
       <c r="O67" t="n">
         <v>0.05838900211188811</v>
       </c>
+      <c r="P67" t="inlineStr">
+        <is>
+          <t>GSVVQEGHD</t>
+        </is>
+      </c>
+      <c r="Q67" t="n">
+        <v>0.05081340777503747</v>
+      </c>
     </row>
     <row r="68">
       <c r="B68" t="inlineStr">
@@ -4416,6 +4928,14 @@
       <c r="O68" t="n">
         <v>0.05833787870097599</v>
       </c>
+      <c r="P68" t="inlineStr">
+        <is>
+          <t>DTTGGDLTE</t>
+        </is>
+      </c>
+      <c r="Q68" t="n">
+        <v>0.05064095776793608</v>
+      </c>
     </row>
     <row r="69">
       <c r="B69" t="inlineStr">
@@ -4474,6 +4994,14 @@
       <c r="O69" t="n">
         <v>0.05830589749264394</v>
       </c>
+      <c r="P69" t="inlineStr">
+        <is>
+          <t>LQEGLTPAA</t>
+        </is>
+      </c>
+      <c r="Q69" t="n">
+        <v>0.05054296987924885</v>
+      </c>
     </row>
     <row r="70">
       <c r="B70" t="inlineStr">
@@ -4532,6 +5060,14 @@
       <c r="O70" t="n">
         <v>0.05827273796254176</v>
       </c>
+      <c r="P70" t="inlineStr">
+        <is>
+          <t>KEGLLGYIE</t>
+        </is>
+      </c>
+      <c r="Q70" t="n">
+        <v>0.05054210270650397</v>
+      </c>
     </row>
     <row r="71">
       <c r="B71" t="inlineStr">
@@ -4590,6 +5126,14 @@
       <c r="O71" t="n">
         <v>0.05808697654424129</v>
       </c>
+      <c r="P71" t="inlineStr">
+        <is>
+          <t>GKTQGEIKG</t>
+        </is>
+      </c>
+      <c r="Q71" t="n">
+        <v>0.05036243234915019</v>
+      </c>
     </row>
     <row r="72">
       <c r="B72" t="inlineStr">
@@ -4648,6 +5192,14 @@
       <c r="O72" t="n">
         <v>0.05801850214978149</v>
       </c>
+      <c r="P72" t="inlineStr">
+        <is>
+          <t>RPKTDTTGG</t>
+        </is>
+      </c>
+      <c r="Q72" t="n">
+        <v>0.05023487554452297</v>
+      </c>
     </row>
     <row r="73">
       <c r="B73" t="inlineStr">
@@ -4706,6 +5258,14 @@
       <c r="O73" t="n">
         <v>0.05798324483171355</v>
       </c>
+      <c r="P73" t="inlineStr">
+        <is>
+          <t>MLAGIYLKV</t>
+        </is>
+      </c>
+      <c r="Q73" t="n">
+        <v>0.05023335775740555</v>
+      </c>
     </row>
     <row r="74">
       <c r="B74" t="inlineStr">
@@ -4764,6 +5324,14 @@
       <c r="O74" t="n">
         <v>0.05797947808791856</v>
       </c>
+      <c r="P74" t="inlineStr">
+        <is>
+          <t>SVVQEGHDG</t>
+        </is>
+      </c>
+      <c r="Q74" t="n">
+        <v>0.05023068113096193</v>
+      </c>
     </row>
     <row r="75">
       <c r="B75" t="inlineStr">
@@ -4822,6 +5390,14 @@
       <c r="O75" t="n">
         <v>0.05783768514441959</v>
       </c>
+      <c r="P75" t="inlineStr">
+        <is>
+          <t>GIKEGLLGY</t>
+        </is>
+      </c>
+      <c r="Q75" t="n">
+        <v>0.05012476252685333</v>
+      </c>
     </row>
     <row r="76">
       <c r="B76" t="inlineStr">
@@ -4880,6 +5456,14 @@
       <c r="O76" t="n">
         <v>0.05783110062330503</v>
       </c>
+      <c r="P76" t="inlineStr">
+        <is>
+          <t>TQGEIKGSV</t>
+        </is>
+      </c>
+      <c r="Q76" t="n">
+        <v>0.05003250019529507</v>
+      </c>
     </row>
     <row r="77">
       <c r="B77" t="inlineStr">
@@ -4938,6 +5522,14 @@
       <c r="O77" t="n">
         <v>0.05780269926746857</v>
       </c>
+      <c r="P77" t="inlineStr">
+        <is>
+          <t>TYKFEKVLI</t>
+        </is>
+      </c>
+      <c r="Q77" t="n">
+        <v>0.0497364164940514</v>
+      </c>
     </row>
     <row r="78">
       <c r="B78" t="inlineStr">
@@ -4996,6 +5588,14 @@
       <c r="O78" t="n">
         <v>0.05772342500601771</v>
       </c>
+      <c r="P78" t="inlineStr">
+        <is>
+          <t>QEGLTPAAA</t>
+        </is>
+      </c>
+      <c r="Q78" t="n">
+        <v>0.04964483531199283</v>
+      </c>
     </row>
     <row r="79">
       <c r="B79" t="inlineStr">
@@ -5054,6 +5654,14 @@
       <c r="O79" t="n">
         <v>0.05768949986833906</v>
       </c>
+      <c r="P79" t="inlineStr">
+        <is>
+          <t>MPARLQEGL</t>
+        </is>
+      </c>
+      <c r="Q79" t="n">
+        <v>0.04962072190563029</v>
+      </c>
     </row>
     <row r="80">
       <c r="B80" t="inlineStr">
@@ -5112,6 +5720,14 @@
       <c r="O80" t="n">
         <v>0.05761161241763968</v>
       </c>
+      <c r="P80" t="inlineStr">
+        <is>
+          <t>EGHDGKIHI</t>
+        </is>
+      </c>
+      <c r="Q80" t="n">
+        <v>0.04942560411861907</v>
+      </c>
     </row>
     <row r="81">
       <c r="B81" t="inlineStr">
@@ -5170,6 +5786,14 @@
       <c r="O81" t="n">
         <v>0.05761065995109259</v>
       </c>
+      <c r="P81" t="inlineStr">
+        <is>
+          <t>IHILAFKND</t>
+        </is>
+      </c>
+      <c r="Q81" t="n">
+        <v>0.0494129134140244</v>
+      </c>
     </row>
     <row r="82">
       <c r="B82" t="inlineStr">
@@ -5228,6 +5852,14 @@
       <c r="O82" t="n">
         <v>0.05758503654212831</v>
       </c>
+      <c r="P82" t="inlineStr">
+        <is>
+          <t>DDSNGIKEG</t>
+        </is>
+      </c>
+      <c r="Q82" t="n">
+        <v>0.04937057248782457</v>
+      </c>
     </row>
     <row r="83">
       <c r="B83" t="inlineStr">
@@ -5286,6 +5918,14 @@
       <c r="O83" t="n">
         <v>0.05755693949745326</v>
       </c>
+      <c r="P83" t="inlineStr">
+        <is>
+          <t>IKEGLLGYI</t>
+        </is>
+      </c>
+      <c r="Q83" t="n">
+        <v>0.04936558150647609</v>
+      </c>
     </row>
     <row r="84">
       <c r="B84" t="inlineStr">
@@ -5344,6 +5984,14 @@
       <c r="O84" t="n">
         <v>0.05749714491010136</v>
       </c>
+      <c r="P84" t="inlineStr">
+        <is>
+          <t>KFEKVLITH</t>
+        </is>
+      </c>
+      <c r="Q84" t="n">
+        <v>0.04930373840721156</v>
+      </c>
     </row>
     <row r="85">
       <c r="B85" t="inlineStr">
@@ -5402,6 +6050,14 @@
       <c r="O85" t="n">
         <v>0.05739023901930457</v>
       </c>
+      <c r="P85" t="inlineStr">
+        <is>
+          <t>KGSVVQEGH</t>
+        </is>
+      </c>
+      <c r="Q85" t="n">
+        <v>0.04917547280310664</v>
+      </c>
     </row>
     <row r="86">
       <c r="B86" t="inlineStr">
@@ -5460,6 +6116,14 @@
       <c r="O86" t="n">
         <v>0.0573725955691551</v>
       </c>
+      <c r="P86" t="inlineStr">
+        <is>
+          <t>DMPARLQEG</t>
+        </is>
+      </c>
+      <c r="Q86" t="n">
+        <v>0.04901001598359366</v>
+      </c>
     </row>
     <row r="87">
       <c r="B87" t="inlineStr">
@@ -5518,6 +6182,14 @@
       <c r="O87" t="n">
         <v>0.05736159791690777</v>
       </c>
+      <c r="P87" t="inlineStr">
+        <is>
+          <t>TELLFTYKF</t>
+        </is>
+      </c>
+      <c r="Q87" t="n">
+        <v>0.04896789469731195</v>
+      </c>
     </row>
     <row r="88">
       <c r="B88" t="inlineStr">
@@ -5576,6 +6248,14 @@
       <c r="O88" t="n">
         <v>0.05733003029646827</v>
       </c>
+      <c r="P88" t="inlineStr">
+        <is>
+          <t>VQEGHDGKI</t>
+        </is>
+      </c>
+      <c r="Q88" t="n">
+        <v>0.04895220676256098</v>
+      </c>
     </row>
     <row r="89">
       <c r="B89" t="inlineStr">
@@ -5634,6 +6314,14 @@
       <c r="O89" t="n">
         <v>0.05721632305306583</v>
       </c>
+      <c r="P89" t="inlineStr">
+        <is>
+          <t>QEGHDGKIH</t>
+        </is>
+      </c>
+      <c r="Q89" t="n">
+        <v>0.048936235318655</v>
+      </c>
     </row>
     <row r="90">
       <c r="B90" t="inlineStr">
@@ -5692,6 +6380,14 @@
       <c r="O90" t="n">
         <v>0.05718160025808813</v>
       </c>
+      <c r="P90" t="inlineStr">
+        <is>
+          <t>KREMMEEFE</t>
+        </is>
+      </c>
+      <c r="Q90" t="n">
+        <v>0.04891559670887716</v>
+      </c>
     </row>
     <row r="91">
       <c r="B91" t="inlineStr">
@@ -5750,6 +6446,14 @@
       <c r="O91" t="n">
         <v>0.05718062160323036</v>
       </c>
+      <c r="P91" t="inlineStr">
+        <is>
+          <t>ARLQEGLTP</t>
+        </is>
+      </c>
+      <c r="Q91" t="n">
+        <v>0.04876689027392193</v>
+      </c>
     </row>
     <row r="92">
       <c r="B92" t="inlineStr">
@@ -5808,6 +6512,14 @@
       <c r="O92" t="n">
         <v>0.05717987730876098</v>
       </c>
+      <c r="P92" t="inlineStr">
+        <is>
+          <t>GTITLTKEM</t>
+        </is>
+      </c>
+      <c r="Q92" t="n">
+        <v>0.04873492687604183</v>
+      </c>
     </row>
     <row r="93">
       <c r="B93" t="inlineStr">
@@ -5866,6 +6578,14 @@
       <c r="O93" t="n">
         <v>0.05717244108376255</v>
       </c>
+      <c r="P93" t="inlineStr">
+        <is>
+          <t>LAGIYLKVK</t>
+        </is>
+      </c>
+      <c r="Q93" t="n">
+        <v>0.04866969260615035</v>
+      </c>
     </row>
     <row r="94">
       <c r="B94" t="inlineStr">
@@ -5924,6 +6644,14 @@
       <c r="O94" t="n">
         <v>0.05710972865053057</v>
       </c>
+      <c r="P94" t="inlineStr">
+        <is>
+          <t>GKREMMEEF</t>
+        </is>
+      </c>
+      <c r="Q94" t="n">
+        <v>0.04833732372850617</v>
+      </c>
     </row>
     <row r="95">
       <c r="B95" t="inlineStr">
@@ -5982,6 +6710,14 @@
       <c r="O95" t="n">
         <v>0.05710923405559586</v>
       </c>
+      <c r="P95" t="inlineStr">
+        <is>
+          <t>PARLQEGLT</t>
+        </is>
+      </c>
+      <c r="Q95" t="n">
+        <v>0.04829101766532597</v>
+      </c>
     </row>
     <row r="96">
       <c r="B96" t="inlineStr">
@@ -6040,6 +6776,14 @@
       <c r="O96" t="n">
         <v>0.05710875862840012</v>
       </c>
+      <c r="P96" t="inlineStr">
+        <is>
+          <t>EIKFAYSGY</t>
+        </is>
+      </c>
+      <c r="Q96" t="n">
+        <v>0.0481120431354161</v>
+      </c>
     </row>
     <row r="97">
       <c r="B97" t="inlineStr">
@@ -6098,6 +6842,14 @@
       <c r="O97" t="n">
         <v>0.05703472603004348</v>
       </c>
+      <c r="P97" t="inlineStr">
+        <is>
+          <t>SPQFLQALG</t>
+        </is>
+      </c>
+      <c r="Q97" t="n">
+        <v>0.04799156836793758</v>
+      </c>
     </row>
     <row r="98">
       <c r="B98" t="inlineStr">
@@ -6156,6 +6908,14 @@
       <c r="O98" t="n">
         <v>0.05701950344880108</v>
       </c>
+      <c r="P98" t="inlineStr">
+        <is>
+          <t>HILAFKNDY</t>
+        </is>
+      </c>
+      <c r="Q98" t="n">
+        <v>0.04798684532876932</v>
+      </c>
     </row>
     <row r="99">
       <c r="B99" t="inlineStr">
@@ -6214,6 +6974,14 @@
       <c r="O99" t="n">
         <v>0.05698619218185937</v>
       </c>
+      <c r="P99" t="inlineStr">
+        <is>
+          <t>NGIKEGLLG</t>
+        </is>
+      </c>
+      <c r="Q99" t="n">
+        <v>0.04773293111605311</v>
+      </c>
     </row>
     <row r="100">
       <c r="B100" t="inlineStr">
@@ -6272,6 +7040,14 @@
       <c r="O100" t="n">
         <v>0.05698163332147432</v>
       </c>
+      <c r="P100" t="inlineStr">
+        <is>
+          <t>HKDDSNGIK</t>
+        </is>
+      </c>
+      <c r="Q100" t="n">
+        <v>0.04760569579498208</v>
+      </c>
     </row>
     <row r="101">
       <c r="B101" t="inlineStr">
@@ -6330,6 +7106,14 @@
       <c r="O101" t="n">
         <v>0.05696324738780086</v>
       </c>
+      <c r="P101" t="inlineStr">
+        <is>
+          <t>ITIHRPKTD</t>
+        </is>
+      </c>
+      <c r="Q101" t="n">
+        <v>0.04756802751254531</v>
+      </c>
     </row>
     <row r="102">
       <c r="B102" t="inlineStr">
@@ -6388,6 +7172,14 @@
       <c r="O102" t="n">
         <v>0.05695682636776464</v>
       </c>
+      <c r="P102" t="inlineStr">
+        <is>
+          <t>SGYSLEHAE</t>
+        </is>
+      </c>
+      <c r="Q102" t="n">
+        <v>0.04749208994787968</v>
+      </c>
     </row>
     <row r="103">
       <c r="B103" t="inlineStr">
@@ -6446,6 +7238,14 @@
       <c r="O103" t="n">
         <v>0.05681845550039789</v>
       </c>
+      <c r="P103" t="inlineStr">
+        <is>
+          <t>ILAFKNDYD</t>
+        </is>
+      </c>
+      <c r="Q103" t="n">
+        <v>0.04726952769060278</v>
+      </c>
     </row>
     <row r="104">
       <c r="B104" t="inlineStr">
@@ -6504,6 +7304,14 @@
       <c r="O104" t="n">
         <v>0.05676076112863433</v>
       </c>
+      <c r="P104" t="inlineStr">
+        <is>
+          <t>LQALGKREM</t>
+        </is>
+      </c>
+      <c r="Q104" t="n">
+        <v>0.04698079926815035</v>
+      </c>
     </row>
     <row r="105">
       <c r="B105" t="inlineStr">
@@ -6562,6 +7370,14 @@
       <c r="O105" t="n">
         <v>0.05672335284785684</v>
       </c>
+      <c r="P105" t="inlineStr">
+        <is>
+          <t>QGEIKGSVV</t>
+        </is>
+      </c>
+      <c r="Q105" t="n">
+        <v>0.04692309443860947</v>
+      </c>
     </row>
     <row r="106">
       <c r="B106" t="inlineStr">
@@ -6620,6 +7436,14 @@
       <c r="O106" t="n">
         <v>0.05671327394314421</v>
       </c>
+      <c r="P106" t="inlineStr">
+        <is>
+          <t>LFTYKFEKV</t>
+        </is>
+      </c>
+      <c r="Q106" t="n">
+        <v>0.04678094256787046</v>
+      </c>
     </row>
     <row r="107">
       <c r="B107" t="inlineStr">
@@ -6678,6 +7502,14 @@
       <c r="O107" t="n">
         <v>0.05669200336490813</v>
       </c>
+      <c r="P107" t="inlineStr">
+        <is>
+          <t>EEIKFAYSG</t>
+        </is>
+      </c>
+      <c r="Q107" t="n">
+        <v>0.0466524042290422</v>
+      </c>
     </row>
     <row r="108">
       <c r="B108" t="inlineStr">
@@ -6736,6 +7568,14 @@
       <c r="O108" t="n">
         <v>0.05668930412663669</v>
       </c>
+      <c r="P108" t="inlineStr">
+        <is>
+          <t>YSGYSLEHA</t>
+        </is>
+      </c>
+      <c r="Q108" t="n">
+        <v>0.04648246124556583</v>
+      </c>
     </row>
     <row r="109">
       <c r="B109" t="inlineStr">
@@ -6794,6 +7634,14 @@
       <c r="O109" t="n">
         <v>0.05660347458905528</v>
       </c>
+      <c r="P109" t="inlineStr">
+        <is>
+          <t>PQFLQALGK</t>
+        </is>
+      </c>
+      <c r="Q109" t="n">
+        <v>0.04646474084183556</v>
+      </c>
     </row>
     <row r="110">
       <c r="B110" t="inlineStr">
@@ -6852,6 +7700,14 @@
       <c r="O110" t="n">
         <v>0.05659031443706131</v>
       </c>
+      <c r="P110" t="inlineStr">
+        <is>
+          <t>IKFAYSGYS</t>
+        </is>
+      </c>
+      <c r="Q110" t="n">
+        <v>0.04646357574431557</v>
+      </c>
     </row>
     <row r="111">
       <c r="B111" t="inlineStr">
@@ -6910,6 +7766,14 @@
       <c r="O111" t="n">
         <v>0.05658732980851325</v>
       </c>
+      <c r="P111" t="inlineStr">
+        <is>
+          <t>FTYKFEKVL</t>
+        </is>
+      </c>
+      <c r="Q111" t="n">
+        <v>0.04631780125602104</v>
+      </c>
     </row>
     <row r="112">
       <c r="B112" t="inlineStr">
@@ -6968,6 +7832,14 @@
       <c r="O112" t="n">
         <v>0.05657456359154312</v>
       </c>
+      <c r="P112" t="inlineStr">
+        <is>
+          <t>YDMPARLQE</t>
+        </is>
+      </c>
+      <c r="Q112" t="n">
+        <v>0.04586157046510425</v>
+      </c>
     </row>
     <row r="113">
       <c r="B113" t="inlineStr">
@@ -7026,6 +7898,14 @@
       <c r="O113" t="n">
         <v>0.05653027959006472</v>
       </c>
+      <c r="P113" t="inlineStr">
+        <is>
+          <t>SSPQFLQAL</t>
+        </is>
+      </c>
+      <c r="Q113" t="n">
+        <v>0.0457632991721247</v>
+      </c>
     </row>
     <row r="114">
       <c r="B114" t="inlineStr">
@@ -7084,6 +7964,14 @@
       <c r="O114" t="n">
         <v>0.05650212013018967</v>
       </c>
+      <c r="P114" t="inlineStr">
+        <is>
+          <t>VLITHMDQY</t>
+        </is>
+      </c>
+      <c r="Q114" t="n">
+        <v>0.04560893748245581</v>
+      </c>
     </row>
     <row r="115">
       <c r="B115" t="inlineStr">
@@ -7142,6 +8030,14 @@
       <c r="O115" t="n">
         <v>0.05647902890982184</v>
       </c>
+      <c r="P115" t="inlineStr">
+        <is>
+          <t>HRPKTDTTG</t>
+        </is>
+      </c>
+      <c r="Q115" t="n">
+        <v>0.04546453880074268</v>
+      </c>
     </row>
     <row r="116">
       <c r="B116" t="inlineStr">
@@ -7200,6 +8096,14 @@
       <c r="O116" t="n">
         <v>0.05643927100611957</v>
       </c>
+      <c r="P116" t="inlineStr">
+        <is>
+          <t>TIHRPKTDT</t>
+        </is>
+      </c>
+      <c r="Q116" t="n">
+        <v>0.04540323165577202</v>
+      </c>
     </row>
     <row r="117">
       <c r="B117" t="inlineStr">
@@ -7258,6 +8162,14 @@
       <c r="O117" t="n">
         <v>0.05643808803977093</v>
       </c>
+      <c r="P117" t="inlineStr">
+        <is>
+          <t>QALGKREMM</t>
+        </is>
+      </c>
+      <c r="Q117" t="n">
+        <v>0.04529440362994468</v>
+      </c>
     </row>
     <row r="118">
       <c r="B118" t="inlineStr">
@@ -7316,6 +8228,14 @@
       <c r="O118" t="n">
         <v>0.05642302934577281</v>
       </c>
+      <c r="P118" t="inlineStr">
+        <is>
+          <t>KDDSNGIKE</t>
+        </is>
+      </c>
+      <c r="Q118" t="n">
+        <v>0.04528918345314785</v>
+      </c>
     </row>
     <row r="119">
       <c r="B119" t="inlineStr">
@@ -7374,6 +8294,14 @@
       <c r="O119" t="n">
         <v>0.0564216212746152</v>
       </c>
+      <c r="P119" t="inlineStr">
+        <is>
+          <t>IKGSVVQEG</t>
+        </is>
+      </c>
+      <c r="Q119" t="n">
+        <v>0.04525827772788377</v>
+      </c>
     </row>
     <row r="120">
       <c r="B120" t="inlineStr">
@@ -7432,6 +8360,14 @@
       <c r="O120" t="n">
         <v>0.05639454013091485</v>
       </c>
+      <c r="P120" t="inlineStr">
+        <is>
+          <t>LGKREMMEE</t>
+        </is>
+      </c>
+      <c r="Q120" t="n">
+        <v>0.04515044681294874</v>
+      </c>
     </row>
     <row r="121">
       <c r="B121" t="inlineStr">
@@ -7490,6 +8426,14 @@
       <c r="O121" t="n">
         <v>0.05638870347783626</v>
       </c>
+      <c r="P121" t="inlineStr">
+        <is>
+          <t>NDYDMPARL</t>
+        </is>
+      </c>
+      <c r="Q121" t="n">
+        <v>0.0450773907189657</v>
+      </c>
     </row>
     <row r="122">
       <c r="B122" t="inlineStr">
@@ -7548,6 +8492,14 @@
       <c r="O122" t="n">
         <v>0.0563866443167546</v>
       </c>
+      <c r="P122" t="inlineStr">
+        <is>
+          <t>DYDMPARLQ</t>
+        </is>
+      </c>
+      <c r="Q122" t="n">
+        <v>0.04485515090829116</v>
+      </c>
     </row>
     <row r="123">
       <c r="B123" t="inlineStr">
@@ -7606,6 +8558,14 @@
       <c r="O123" t="n">
         <v>0.05638630980801662</v>
       </c>
+      <c r="P123" t="inlineStr">
+        <is>
+          <t>YSPTPHKDD</t>
+        </is>
+      </c>
+      <c r="Q123" t="n">
+        <v>0.0448389168486306</v>
+      </c>
     </row>
     <row r="124">
       <c r="B124" t="inlineStr">
@@ -7664,6 +8624,14 @@
       <c r="O124" t="n">
         <v>0.05632939525504305</v>
       </c>
+      <c r="P124" t="inlineStr">
+        <is>
+          <t>IHRPKTDTT</t>
+        </is>
+      </c>
+      <c r="Q124" t="n">
+        <v>0.04473156556997555</v>
+      </c>
     </row>
     <row r="125">
       <c r="B125" t="inlineStr">
@@ -7722,6 +8690,14 @@
       <c r="O125" t="n">
         <v>0.05632127187030714</v>
       </c>
+      <c r="P125" t="inlineStr">
+        <is>
+          <t>FLQALGKRE</t>
+        </is>
+      </c>
+      <c r="Q125" t="n">
+        <v>0.04463301604647513</v>
+      </c>
     </row>
     <row r="126">
       <c r="B126" t="inlineStr">
@@ -7780,6 +8756,14 @@
       <c r="O126" t="n">
         <v>0.05628731599904196</v>
       </c>
+      <c r="P126" t="inlineStr">
+        <is>
+          <t>LTKEMDRSS</t>
+        </is>
+      </c>
+      <c r="Q126" t="n">
+        <v>0.04453556344412189</v>
+      </c>
     </row>
     <row r="127">
       <c r="B127" t="inlineStr">
@@ -7838,6 +8822,14 @@
       <c r="O127" t="n">
         <v>0.05625155745381244</v>
       </c>
+      <c r="P127" t="inlineStr">
+        <is>
+          <t>AYSGYSLEH</t>
+        </is>
+      </c>
+      <c r="Q127" t="n">
+        <v>0.04445657749934873</v>
+      </c>
     </row>
     <row r="128">
       <c r="B128" t="inlineStr">
@@ -7896,6 +8888,14 @@
       <c r="O128" t="n">
         <v>0.05624273244935009</v>
       </c>
+      <c r="P128" t="inlineStr">
+        <is>
+          <t>SPTPHKDDS</t>
+        </is>
+      </c>
+      <c r="Q128" t="n">
+        <v>0.04420300093786664</v>
+      </c>
     </row>
     <row r="129">
       <c r="B129" t="inlineStr">
@@ -7954,6 +8954,14 @@
       <c r="O129" t="n">
         <v>0.05622082463887614</v>
       </c>
+      <c r="P129" t="inlineStr">
+        <is>
+          <t>RSSPQFLQA</t>
+        </is>
+      </c>
+      <c r="Q129" t="n">
+        <v>0.04418316447818018</v>
+      </c>
     </row>
     <row r="130">
       <c r="B130" t="inlineStr">
@@ -8012,6 +9020,14 @@
       <c r="O130" t="n">
         <v>0.05616943139927972</v>
       </c>
+      <c r="P130" t="inlineStr">
+        <is>
+          <t>FKNDYDMPA</t>
+        </is>
+      </c>
+      <c r="Q130" t="n">
+        <v>0.04411445151791293</v>
+      </c>
     </row>
     <row r="131">
       <c r="B131" t="inlineStr">
@@ -8070,6 +9086,14 @@
       <c r="O131" t="n">
         <v>0.05616748589403908</v>
       </c>
+      <c r="P131" t="inlineStr">
+        <is>
+          <t>TITLTKEMD</t>
+        </is>
+      </c>
+      <c r="Q131" t="n">
+        <v>0.04406887615833776</v>
+      </c>
     </row>
     <row r="132">
       <c r="B132" t="inlineStr">
@@ -8128,6 +9152,14 @@
       <c r="O132" t="n">
         <v>0.05616437966806943</v>
       </c>
+      <c r="P132" t="inlineStr">
+        <is>
+          <t>LAFKNDYDM</t>
+        </is>
+      </c>
+      <c r="Q132" t="n">
+        <v>0.04398837561251283</v>
+      </c>
     </row>
     <row r="133">
       <c r="B133" t="inlineStr">
@@ -8186,6 +9218,14 @@
       <c r="O133" t="n">
         <v>0.05614650565788091</v>
       </c>
+      <c r="P133" t="inlineStr">
+        <is>
+          <t>QYSPTPHKD</t>
+        </is>
+      </c>
+      <c r="Q133" t="n">
+        <v>0.04398080381280432</v>
+      </c>
     </row>
     <row r="134">
       <c r="B134" t="inlineStr">
@@ -8244,6 +9284,14 @@
       <c r="O134" t="n">
         <v>0.056079879505004</v>
       </c>
+      <c r="P134" t="inlineStr">
+        <is>
+          <t>KNDYDMPAR</t>
+        </is>
+      </c>
+      <c r="Q134" t="n">
+        <v>0.04396975525805932</v>
+      </c>
     </row>
     <row r="135">
       <c r="B135" t="inlineStr">
@@ -8302,6 +9350,14 @@
       <c r="O135" t="n">
         <v>0.05604005515092692</v>
       </c>
+      <c r="P135" t="inlineStr">
+        <is>
+          <t>DQYSPTPHK</t>
+        </is>
+      </c>
+      <c r="Q135" t="n">
+        <v>0.04376608378560849</v>
+      </c>
     </row>
     <row r="136">
       <c r="B136" t="inlineStr">
@@ -8360,6 +9416,14 @@
       <c r="O136" t="n">
         <v>0.05603284378601345</v>
       </c>
+      <c r="P136" t="inlineStr">
+        <is>
+          <t>VKGKTQGEI</t>
+        </is>
+      </c>
+      <c r="Q136" t="n">
+        <v>0.04361218671343957</v>
+      </c>
     </row>
     <row r="137">
       <c r="B137" t="inlineStr">
@@ -8418,6 +9482,14 @@
       <c r="O137" t="n">
         <v>0.05600927801450847</v>
       </c>
+      <c r="P137" t="inlineStr">
+        <is>
+          <t>AFKNDYDMP</t>
+        </is>
+      </c>
+      <c r="Q137" t="n">
+        <v>0.04358079566780454</v>
+      </c>
     </row>
     <row r="138">
       <c r="B138" t="inlineStr">
@@ -8476,6 +9548,14 @@
       <c r="O138" t="n">
         <v>0.05600694904241539</v>
       </c>
+      <c r="P138" t="inlineStr">
+        <is>
+          <t>TLTKEMDRS</t>
+        </is>
+      </c>
+      <c r="Q138" t="n">
+        <v>0.04343680118369748</v>
+      </c>
     </row>
     <row r="139">
       <c r="B139" t="inlineStr">
@@ -8534,6 +9614,14 @@
       <c r="O139" t="n">
         <v>0.05600629394956128</v>
       </c>
+      <c r="P139" t="inlineStr">
+        <is>
+          <t>ITLTKEMDR</t>
+        </is>
+      </c>
+      <c r="Q139" t="n">
+        <v>0.04343648794603256</v>
+      </c>
     </row>
     <row r="140">
       <c r="B140" t="inlineStr">
@@ -8592,6 +9680,14 @@
       <c r="O140" t="n">
         <v>0.05597822581630692</v>
       </c>
+      <c r="P140" t="inlineStr">
+        <is>
+          <t>PHKDDSNGI</t>
+        </is>
+      </c>
+      <c r="Q140" t="n">
+        <v>0.04315487687649518</v>
+      </c>
     </row>
     <row r="141">
       <c r="B141" t="inlineStr">
@@ -8650,6 +9746,14 @@
       <c r="O141" t="n">
         <v>0.05597803346800266</v>
       </c>
+      <c r="P141" t="inlineStr">
+        <is>
+          <t>EIKGSVVQE</t>
+        </is>
+      </c>
+      <c r="Q141" t="n">
+        <v>0.0429368338646928</v>
+      </c>
     </row>
     <row r="142">
       <c r="B142" t="inlineStr">
@@ -8708,6 +9812,14 @@
       <c r="O142" t="n">
         <v>0.05594956112644275</v>
       </c>
+      <c r="P142" t="inlineStr">
+        <is>
+          <t>GEIKGSVVQ</t>
+        </is>
+      </c>
+      <c r="Q142" t="n">
+        <v>0.04267558189027705</v>
+      </c>
     </row>
     <row r="143">
       <c r="B143" t="inlineStr">
@@ -8766,6 +9878,14 @@
       <c r="O143" t="n">
         <v>0.05594841959977857</v>
       </c>
+      <c r="P143" t="inlineStr">
+        <is>
+          <t>QFLQALGKR</t>
+        </is>
+      </c>
+      <c r="Q143" t="n">
+        <v>0.04247584612159816</v>
+      </c>
     </row>
     <row r="144">
       <c r="B144" t="inlineStr">
@@ -8824,6 +9944,14 @@
       <c r="O144" t="n">
         <v>0.05586296018871267</v>
       </c>
+      <c r="P144" t="inlineStr">
+        <is>
+          <t>MDQYSPTPH</t>
+        </is>
+      </c>
+      <c r="Q144" t="n">
+        <v>0.04212895734196687</v>
+      </c>
     </row>
     <row r="145">
       <c r="B145" t="inlineStr">
@@ -8882,6 +10010,14 @@
       <c r="O145" t="n">
         <v>0.05582544503094442</v>
       </c>
+      <c r="P145" t="inlineStr">
+        <is>
+          <t>LITHMDQYS</t>
+        </is>
+      </c>
+      <c r="Q145" t="n">
+        <v>0.04202576688413191</v>
+      </c>
     </row>
     <row r="146">
       <c r="B146" t="inlineStr">
@@ -8940,6 +10076,14 @@
       <c r="O146" t="n">
         <v>0.05577699572930722</v>
       </c>
+      <c r="P146" t="inlineStr">
+        <is>
+          <t>PTPHKDDSN</t>
+        </is>
+      </c>
+      <c r="Q146" t="n">
+        <v>0.04172096084857192</v>
+      </c>
     </row>
     <row r="147">
       <c r="B147" t="inlineStr">
@@ -8998,6 +10142,14 @@
       <c r="O147" t="n">
         <v>0.05577489339284727</v>
       </c>
+      <c r="P147" t="inlineStr">
+        <is>
+          <t>DRSSPQFLQ</t>
+        </is>
+      </c>
+      <c r="Q147" t="n">
+        <v>0.04158958702340361</v>
+      </c>
     </row>
     <row r="148">
       <c r="B148" t="inlineStr">
@@ -9056,6 +10208,14 @@
       <c r="O148" t="n">
         <v>0.05577280166096343</v>
       </c>
+      <c r="P148" t="inlineStr">
+        <is>
+          <t>KFAYSGYSL</t>
+        </is>
+      </c>
+      <c r="Q148" t="n">
+        <v>0.04155851265711533</v>
+      </c>
     </row>
     <row r="149">
       <c r="B149" t="inlineStr">
@@ -9114,6 +10274,14 @@
       <c r="O149" t="n">
         <v>0.05576825355041906</v>
       </c>
+      <c r="P149" t="inlineStr">
+        <is>
+          <t>AGIYLKVKG</t>
+        </is>
+      </c>
+      <c r="Q149" t="n">
+        <v>0.041538472119402</v>
+      </c>
     </row>
     <row r="150">
       <c r="B150" t="inlineStr">
@@ -9172,6 +10340,14 @@
       <c r="O150" t="n">
         <v>0.05575481423938459</v>
       </c>
+      <c r="P150" t="inlineStr">
+        <is>
+          <t>ALGKREMME</t>
+        </is>
+      </c>
+      <c r="Q150" t="n">
+        <v>0.04122201205667409</v>
+      </c>
     </row>
     <row r="151">
       <c r="B151" t="inlineStr">
@@ -9230,6 +10406,14 @@
       <c r="O151" t="n">
         <v>0.05572850316520431</v>
       </c>
+      <c r="P151" t="inlineStr">
+        <is>
+          <t>KVKGKTQGE</t>
+        </is>
+      </c>
+      <c r="Q151" t="n">
+        <v>0.04065163881207413</v>
+      </c>
     </row>
     <row r="152">
       <c r="B152" t="inlineStr">
@@ -9288,6 +10472,14 @@
       <c r="O152" t="n">
         <v>0.05570858815431859</v>
       </c>
+      <c r="P152" t="inlineStr">
+        <is>
+          <t>HMDQYSPTP</t>
+        </is>
+      </c>
+      <c r="Q152" t="n">
+        <v>0.04026710684926018</v>
+      </c>
     </row>
     <row r="153">
       <c r="B153" t="inlineStr">
@@ -9346,6 +10538,14 @@
       <c r="O153" t="n">
         <v>0.0556999538198021</v>
       </c>
+      <c r="P153" t="inlineStr">
+        <is>
+          <t>KEMDRSSPQ</t>
+        </is>
+      </c>
+      <c r="Q153" t="n">
+        <v>0.04021749284390257</v>
+      </c>
     </row>
     <row r="154">
       <c r="B154" t="inlineStr">
@@ -9404,6 +10604,14 @@
       <c r="O154" t="n">
         <v>0.05569038145115398</v>
       </c>
+      <c r="P154" t="inlineStr">
+        <is>
+          <t>TKEMDRSSP</t>
+        </is>
+      </c>
+      <c r="Q154" t="n">
+        <v>0.04010905109276046</v>
+      </c>
     </row>
     <row r="155">
       <c r="B155" t="inlineStr">
@@ -9462,6 +10670,14 @@
       <c r="O155" t="n">
         <v>0.05567037927675743</v>
       </c>
+      <c r="P155" t="inlineStr">
+        <is>
+          <t>TPHKDDSNG</t>
+        </is>
+      </c>
+      <c r="Q155" t="n">
+        <v>0.03981527750617909</v>
+      </c>
     </row>
     <row r="156">
       <c r="B156" t="inlineStr">
@@ -9520,6 +10736,14 @@
       <c r="O156" t="n">
         <v>0.05563398223784233</v>
       </c>
+      <c r="P156" t="inlineStr">
+        <is>
+          <t>FAYSGYSLE</t>
+        </is>
+      </c>
+      <c r="Q156" t="n">
+        <v>0.03980693344526509</v>
+      </c>
     </row>
     <row r="157">
       <c r="B157" t="inlineStr">
@@ -9578,6 +10802,14 @@
       <c r="O157" t="n">
         <v>0.05562106265310847</v>
       </c>
+      <c r="P157" t="inlineStr">
+        <is>
+          <t>YLKVKGKTQ</t>
+        </is>
+      </c>
+      <c r="Q157" t="n">
+        <v>0.03925731855386381</v>
+      </c>
     </row>
     <row r="158">
       <c r="B158" t="inlineStr">
@@ -9636,6 +10868,14 @@
       <c r="O158" t="n">
         <v>0.05561309560453299</v>
       </c>
+      <c r="P158" t="inlineStr">
+        <is>
+          <t>GIYLKVKGK</t>
+        </is>
+      </c>
+      <c r="Q158" t="n">
+        <v>0.03920404601284776</v>
+      </c>
     </row>
     <row r="159">
       <c r="B159" t="inlineStr">
@@ -9694,6 +10934,14 @@
       <c r="O159" t="n">
         <v>0.05557709184540473</v>
       </c>
+      <c r="P159" t="inlineStr">
+        <is>
+          <t>THMDQYSPT</t>
+        </is>
+      </c>
+      <c r="Q159" t="n">
+        <v>0.03918376409960991</v>
+      </c>
     </row>
     <row r="160">
       <c r="B160" t="inlineStr">
@@ -9752,6 +11000,14 @@
       <c r="O160" t="n">
         <v>0.05552505848647688</v>
       </c>
+      <c r="P160" t="inlineStr">
+        <is>
+          <t>MDRSSPQFL</t>
+        </is>
+      </c>
+      <c r="Q160" t="n">
+        <v>0.03881034176952239</v>
+      </c>
     </row>
     <row r="161">
       <c r="B161" t="inlineStr">
@@ -9810,6 +11066,14 @@
       <c r="O161" t="n">
         <v>0.0555137720960294</v>
       </c>
+      <c r="P161" t="inlineStr">
+        <is>
+          <t>EMDRSSPQF</t>
+        </is>
+      </c>
+      <c r="Q161" t="n">
+        <v>0.03871670275234826</v>
+      </c>
     </row>
     <row r="162">
       <c r="B162" t="inlineStr">
@@ -9868,6 +11132,14 @@
       <c r="O162" t="n">
         <v>0.05548965522676737</v>
       </c>
+      <c r="P162" t="inlineStr">
+        <is>
+          <t>ITHMDQYSP</t>
+        </is>
+      </c>
+      <c r="Q162" t="n">
+        <v>0.03795686873921085</v>
+      </c>
     </row>
     <row r="163">
       <c r="B163" t="inlineStr">
@@ -9926,6 +11198,14 @@
       <c r="O163" t="n">
         <v>0.05547803469007312</v>
       </c>
+      <c r="P163" t="inlineStr">
+        <is>
+          <t>LKVKGKTQG</t>
+        </is>
+      </c>
+      <c r="Q163" t="n">
+        <v>0.03781645974983729</v>
+      </c>
     </row>
     <row r="164">
       <c r="B164" t="inlineStr">
@@ -9983,6 +11263,14 @@
       </c>
       <c r="O164" t="n">
         <v>0.05542402401048445</v>
+      </c>
+      <c r="P164" t="inlineStr">
+        <is>
+          <t>IYLKVKGKT</t>
+        </is>
+      </c>
+      <c r="Q164" t="n">
+        <v>0.03623898512546719</v>
       </c>
     </row>
     <row r="165">

</xml_diff>